<commit_message>
remove "user-specific" from example rows
</commit_message>
<xml_diff>
--- a/templates/community/TRR341_Phenotyping/Study_Watering_protocol_TRR341_MIAPPE.xlsx
+++ b/templates/community/TRR341_Phenotyping/Study_Watering_protocol_TRR341_MIAPPE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julie Jacquemin\Documents\GitHub\Swate-templates_myfork\templates\community\TRR341_Phenotyping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/TRR341_Phenotyping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81EC3FC-44A7-4E78-BC39-FB04CF361A1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A1BF6-A8D2-DC40-8B40-3CD28503CFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1875" yWindow="1830" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{78A6E57C-3BF1-47BC-BB84-15DDB1AF3B29}"/>
+    <workbookView xWindow="1860" yWindow="1840" windowWidth="21600" windowHeight="11380" xr2:uid="{78A6E57C-3BF1-47BC-BB84-15DDB1AF3B29}"/>
   </bookViews>
   <sheets>
     <sheet name="Watering_protocol" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>Watering</t>
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>user-specific</t>
   </si>
   <si>
     <t>Sample Name</t>
@@ -774,70 +771,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00CB69D-2356-429D-8304-F8A1FB5648BF}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="26" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="24.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
@@ -857,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -870,7 +863,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -883,7 +876,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
@@ -896,7 +889,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -909,7 +902,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>0</v>
       </c>
@@ -922,7 +915,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -935,7 +928,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +941,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
@@ -961,7 +954,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,6 +969,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -986,217 +980,217 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD94F2F-7537-4E24-852F-032F10D799F9}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="65.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="65.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B2" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B17" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="3"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="3"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20" s="3"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="3"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="3"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>40</v>
       </c>
       <c r="B27" s="9"/>
     </row>

</xml_diff>

<commit_message>
[test] test - trigger swobup
</commit_message>
<xml_diff>
--- a/templates/community/TRR341_Phenotyping/Study_Watering_protocol_TRR341_MIAPPE.xlsx
+++ b/templates/community/TRR341_Phenotyping/Study_Watering_protocol_TRR341_MIAPPE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/TRR341_Phenotyping/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1A1BF6-A8D2-DC40-8B40-3CD28503CFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D826FF8-BD95-CB46-A627-2D4711891604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1840" windowWidth="21600" windowHeight="11380" xr2:uid="{78A6E57C-3BF1-47BC-BB84-15DDB1AF3B29}"/>
+    <workbookView xWindow="1860" yWindow="1840" windowWidth="21600" windowHeight="11380" activeTab="1" xr2:uid="{78A6E57C-3BF1-47BC-BB84-15DDB1AF3B29}"/>
   </bookViews>
   <sheets>
     <sheet name="Watering_protocol" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>d088bf2c-a6e1-4bea-b428-ca1c6646c60a</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Watering protocol for Study file MIAPPE</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>MIAPPE</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
   </si>
 </sst>
 </file>
@@ -771,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00CB69D-2356-429D-8304-F8A1FB5648BF}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="C2:D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -980,8 +980,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD94F2F-7537-4E24-852F-032F10D799F9}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1003,7 +1003,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -1011,7 +1011,7 @@
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -1019,7 +1019,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
         <v>17</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -1035,7 +1035,7 @@
         <v>18</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1073,25 +1073,25 @@
         <v>24</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>53</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>54</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>56</v>
-      </c>
-      <c r="H12" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1117,7 +1117,7 @@
         <v>28</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -1125,7 +1125,7 @@
         <v>29</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -1139,7 +1139,7 @@
         <v>31</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1165,7 +1165,7 @@
         <v>35</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -1179,7 +1179,7 @@
         <v>37</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>